<commit_message>
New datasets in 3 different formats
</commit_message>
<xml_diff>
--- a/input/3Var_Linear1.xlsx
+++ b/input/3Var_Linear1.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -470,19 +470,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2343197618734421</v>
+        <v>0.174591510220848</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2227004909697526</v>
+        <v>0.1258683508400295</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5044311418976827</v>
+        <v>1.155256459293242</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2493825440359637</v>
+        <v>0.1822841748126243</v>
       </c>
     </row>
     <row r="3">
@@ -490,19 +490,19 @@
         <v>0.5263157894736842</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2912111269809378</v>
+        <v>0.2954516743906898</v>
       </c>
       <c r="C3" t="n">
         <v>0.2631578947368421</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1520286203760581</v>
+        <v>0.1361460328409026</v>
       </c>
       <c r="E3" t="n">
-        <v>2.188977345138301</v>
+        <v>2.949074107730708</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2719975959692685</v>
+        <v>0.29878681355207</v>
       </c>
     </row>
     <row r="4">
@@ -510,19 +510,19 @@
         <v>1.052631578947368</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1397303481840248</v>
+        <v>0.2855239290104701</v>
       </c>
       <c r="C4" t="n">
         <v>0.5263157894736842</v>
       </c>
       <c r="D4" t="n">
-        <v>0.08544772716552967</v>
+        <v>0.1736533016683439</v>
       </c>
       <c r="E4" t="n">
-        <v>4.660604374209584</v>
+        <v>3.666211514761394</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3426918217453939</v>
+        <v>0.2230009963955268</v>
       </c>
     </row>
     <row r="5">
@@ -530,19 +530,19 @@
         <v>1.578947368421053</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2055633484348907</v>
+        <v>0.1243648165791852</v>
       </c>
       <c r="C5" t="n">
         <v>0.7894736842105263</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1923226172900212</v>
+        <v>0.114408573474128</v>
       </c>
       <c r="E5" t="n">
-        <v>5.876234472937544</v>
+        <v>6.42049203935059</v>
       </c>
       <c r="F5" t="n">
-        <v>0.3381301858119656</v>
+        <v>0.1749400651923788</v>
       </c>
     </row>
     <row r="6">
@@ -550,19 +550,19 @@
         <v>2.105263157894737</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2460375484203127</v>
+        <v>0.255523429346789</v>
       </c>
       <c r="C6" t="n">
         <v>1.052631578947368</v>
       </c>
       <c r="D6" t="n">
-        <v>0.1646443385668269</v>
+        <v>0.1501314074596035</v>
       </c>
       <c r="E6" t="n">
-        <v>8.085053859262112</v>
+        <v>8.770462758967463</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1521032590351934</v>
+        <v>0.3770581559129562</v>
       </c>
     </row>
     <row r="7">
@@ -570,19 +570,19 @@
         <v>2.631578947368421</v>
       </c>
       <c r="B7" t="n">
-        <v>0.1877754877184833</v>
+        <v>0.2540495197352055</v>
       </c>
       <c r="C7" t="n">
         <v>1.31578947368421</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1259750855378525</v>
+        <v>0.09049827347454925</v>
       </c>
       <c r="E7" t="n">
-        <v>10.41410955450997</v>
+        <v>9.727841100460605</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1808380201015198</v>
+        <v>0.1928717669813325</v>
       </c>
     </row>
     <row r="8">
@@ -590,19 +590,19 @@
         <v>3.157894736842105</v>
       </c>
       <c r="B8" t="n">
-        <v>0.2377710430811885</v>
+        <v>0.1494001570811972</v>
       </c>
       <c r="C8" t="n">
         <v>1.578947368421053</v>
       </c>
       <c r="D8" t="n">
-        <v>0.09969925460412055</v>
+        <v>0.1334653984824515</v>
       </c>
       <c r="E8" t="n">
-        <v>11.92733223544565</v>
+        <v>12.46071583139859</v>
       </c>
       <c r="F8" t="n">
-        <v>0.3180565436650487</v>
+        <v>0.3121757356295127</v>
       </c>
     </row>
     <row r="9">
@@ -610,19 +610,19 @@
         <v>3.684210526315789</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1723301385953339</v>
+        <v>0.2703745199553737</v>
       </c>
       <c r="C9" t="n">
         <v>1.842105263157895</v>
       </c>
       <c r="D9" t="n">
-        <v>0.133562307225647</v>
+        <v>0.1392095412808186</v>
       </c>
       <c r="E9" t="n">
-        <v>14.35174024967534</v>
+        <v>14.69817297899096</v>
       </c>
       <c r="F9" t="n">
-        <v>0.3692868103004107</v>
+        <v>0.2863203349234984</v>
       </c>
     </row>
     <row r="10">
@@ -630,19 +630,19 @@
         <v>4.210526315789473</v>
       </c>
       <c r="B10" t="n">
-        <v>0.1228691085818852</v>
+        <v>0.1593764287736224</v>
       </c>
       <c r="C10" t="n">
         <v>2.105263157894737</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1211147781765214</v>
+        <v>0.09586511171837554</v>
       </c>
       <c r="E10" t="n">
-        <v>16.17452188205988</v>
+        <v>15.28109735322164</v>
       </c>
       <c r="F10" t="n">
-        <v>0.3037267523285127</v>
+        <v>0.3658404188637184</v>
       </c>
     </row>
     <row r="11">
@@ -650,19 +650,19 @@
         <v>4.736842105263158</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1013531377514409</v>
+        <v>0.2835086356192502</v>
       </c>
       <c r="C11" t="n">
         <v>2.368421052631579</v>
       </c>
       <c r="D11" t="n">
-        <v>0.1893766425276281</v>
+        <v>0.09788018914535139</v>
       </c>
       <c r="E11" t="n">
-        <v>17.63158587821708</v>
+        <v>17.54154182639366</v>
       </c>
       <c r="F11" t="n">
-        <v>0.3667846972102187</v>
+        <v>0.3052147677044286</v>
       </c>
     </row>
     <row r="12">
@@ -670,19 +670,19 @@
         <v>5.263157894736842</v>
       </c>
       <c r="B12" t="n">
-        <v>0.1807281719731974</v>
+        <v>0.1262559437430216</v>
       </c>
       <c r="C12" t="n">
         <v>2.631578947368421</v>
       </c>
       <c r="D12" t="n">
-        <v>0.09547719650528132</v>
+        <v>0.1864472475251674</v>
       </c>
       <c r="E12" t="n">
-        <v>19.60722357455633</v>
+        <v>19.37303394764616</v>
       </c>
       <c r="F12" t="n">
-        <v>0.3432261683424848</v>
+        <v>0.3943487833754562</v>
       </c>
     </row>
     <row r="13">
@@ -690,19 +690,19 @@
         <v>5.789473684210526</v>
       </c>
       <c r="B13" t="n">
-        <v>0.2459025333887607</v>
+        <v>0.1107120942924899</v>
       </c>
       <c r="C13" t="n">
         <v>2.894736842105263</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1369455424946706</v>
+        <v>0.0960975017415991</v>
       </c>
       <c r="E13" t="n">
-        <v>20.91816383261152</v>
+        <v>20.73823033391738</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1620436711928101</v>
+        <v>0.1751770002859284</v>
       </c>
     </row>
     <row r="14">
@@ -710,19 +710,19 @@
         <v>6.315789473684211</v>
       </c>
       <c r="B14" t="n">
-        <v>0.2187035789679521</v>
+        <v>0.2814512366711349</v>
       </c>
       <c r="C14" t="n">
         <v>3.157894736842105</v>
       </c>
       <c r="D14" t="n">
-        <v>0.1963311126091059</v>
+        <v>0.1352677896355402</v>
       </c>
       <c r="E14" t="n">
-        <v>23.12462436828154</v>
+        <v>21.69196349552623</v>
       </c>
       <c r="F14" t="n">
-        <v>0.2779458159617622</v>
+        <v>0.3385760466189176</v>
       </c>
     </row>
     <row r="15">
@@ -730,19 +730,19 @@
         <v>6.842105263157895</v>
       </c>
       <c r="B15" t="n">
-        <v>0.282801648483775</v>
+        <v>0.2430667063229389</v>
       </c>
       <c r="C15" t="n">
         <v>3.421052631578947</v>
       </c>
       <c r="D15" t="n">
-        <v>0.1936365555481474</v>
+        <v>0.1480316964732308</v>
       </c>
       <c r="E15" t="n">
-        <v>25.23449884961524</v>
+        <v>25.69722107590501</v>
       </c>
       <c r="F15" t="n">
-        <v>0.39771320360347</v>
+        <v>0.4142887397523345</v>
       </c>
     </row>
     <row r="16">
@@ -750,19 +750,19 @@
         <v>7.368421052631579</v>
       </c>
       <c r="B16" t="n">
-        <v>0.2639960925514754</v>
+        <v>0.2326655413894682</v>
       </c>
       <c r="C16" t="n">
         <v>3.684210526315789</v>
       </c>
       <c r="D16" t="n">
-        <v>0.2142319414253331</v>
+        <v>0.1205392373751327</v>
       </c>
       <c r="E16" t="n">
-        <v>26.64533648327219</v>
+        <v>27.0195648418906</v>
       </c>
       <c r="F16" t="n">
-        <v>0.3184417846414749</v>
+        <v>0.2819937502787892</v>
       </c>
     </row>
     <row r="17">
@@ -770,19 +770,19 @@
         <v>7.894736842105263</v>
       </c>
       <c r="B17" t="n">
-        <v>0.2360924922090135</v>
+        <v>0.1901363180535316</v>
       </c>
       <c r="C17" t="n">
         <v>3.947368421052631</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1589818535728771</v>
+        <v>0.09588772143902059</v>
       </c>
       <c r="E17" t="n">
-        <v>29.20782779670689</v>
+        <v>29.58556960858154</v>
       </c>
       <c r="F17" t="n">
-        <v>0.358586406138433</v>
+        <v>0.1834109107854891</v>
       </c>
     </row>
     <row r="18">
@@ -790,19 +790,19 @@
         <v>8.421052631578947</v>
       </c>
       <c r="B18" t="n">
-        <v>0.2589174167197018</v>
+        <v>0.1435525429874498</v>
       </c>
       <c r="C18" t="n">
         <v>4.210526315789473</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1380736178524921</v>
+        <v>0.1372984624797285</v>
       </c>
       <c r="E18" t="n">
-        <v>30.05867423090865</v>
+        <v>30.19963124694031</v>
       </c>
       <c r="F18" t="n">
-        <v>0.2318826979153745</v>
+        <v>0.2613003229174928</v>
       </c>
     </row>
     <row r="19">
@@ -810,19 +810,19 @@
         <v>8.947368421052632</v>
       </c>
       <c r="B19" t="n">
-        <v>0.1638869612482384</v>
+        <v>0.1708694871536545</v>
       </c>
       <c r="C19" t="n">
         <v>4.473684210526316</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1912388108520984</v>
+        <v>0.1496943840011644</v>
       </c>
       <c r="E19" t="n">
-        <v>32.43438493940538</v>
+        <v>32.85293938245817</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4032426239811157</v>
+        <v>0.3886537178955867</v>
       </c>
     </row>
     <row r="20">
@@ -830,19 +830,19 @@
         <v>9.473684210526315</v>
       </c>
       <c r="B20" t="n">
-        <v>0.2904857786499359</v>
+        <v>0.2604398570439498</v>
       </c>
       <c r="C20" t="n">
         <v>4.736842105263158</v>
       </c>
       <c r="D20" t="n">
-        <v>0.2013807379245006</v>
+        <v>0.2025188775800254</v>
       </c>
       <c r="E20" t="n">
-        <v>34.22592971622102</v>
+        <v>35.18952747146144</v>
       </c>
       <c r="F20" t="n">
-        <v>0.2358704334739168</v>
+        <v>0.4313863417107523</v>
       </c>
     </row>
     <row r="21">
@@ -850,19 +850,19 @@
         <v>10</v>
       </c>
       <c r="B21" t="n">
-        <v>0.1199551239822736</v>
+        <v>0.1030433709033476</v>
       </c>
       <c r="C21" t="n">
         <v>5</v>
       </c>
       <c r="D21" t="n">
-        <v>0.1058862725326557</v>
+        <v>0.1674002993442782</v>
       </c>
       <c r="E21" t="n">
-        <v>36.167371262025</v>
+        <v>35.62434345300911</v>
       </c>
       <c r="F21" t="n">
-        <v>0.3714134584426688</v>
+        <v>0.4426611090471849</v>
       </c>
     </row>
   </sheetData>

</xml_diff>